<commit_message>
update note of English
</commit_message>
<xml_diff>
--- a/Words/Mispronounced words.xlsx
+++ b/Words/Mispronounced words.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Private Files\English Note\Words\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA4E4E21-0224-4D48-B066-18EDB8E0B715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C7E51B-4158-456D-91DC-F607B31D052E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Words</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -84,13 +84,175 @@
   </si>
   <si>
     <t>/ˈkwɪə.ri/</t>
+  </si>
+  <si>
+    <t>specific</t>
+  </si>
+  <si>
+    <r>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="GWIPA"/>
+        <charset val="2"/>
+      </rPr>
+      <t>spE'sIfIk</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/</t>
+    </r>
+  </si>
+  <si>
+    <t>niche</t>
+  </si>
+  <si>
+    <r>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="GWIPA"/>
+        <charset val="2"/>
+      </rPr>
+      <t>ni:S</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/</t>
+    </r>
+  </si>
+  <si>
+    <t>bargaining</t>
+  </si>
+  <si>
+    <r>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="GWIPA"/>
+        <charset val="2"/>
+      </rPr>
+      <t>'bA:gEnIN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/</t>
+    </r>
+  </si>
+  <si>
+    <t>[U.]</t>
+  </si>
+  <si>
+    <t>suite</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /swi:t/ </t>
+  </si>
+  <si>
+    <t>automate</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /'O:tEmeIt/ </t>
+  </si>
+  <si>
+    <t>n.</t>
+  </si>
+  <si>
+    <t>vt.</t>
+  </si>
+  <si>
+    <t>modular</t>
+  </si>
+  <si>
+    <r>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="GWIPA"/>
+        <charset val="2"/>
+      </rPr>
+      <t>'mOdjulE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/</t>
+    </r>
+  </si>
+  <si>
+    <t>adj.</t>
+  </si>
+  <si>
+    <t>character</t>
+  </si>
+  <si>
+    <r>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="GWIPA"/>
+        <charset val="2"/>
+      </rPr>
+      <t>'kQrEktE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/</t>
+    </r>
+  </si>
+  <si>
+    <t>n.single</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,6 +280,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="GWIPA"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -127,7 +301,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -150,11 +324,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -167,9 +365,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -450,14 +653,14 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" customHeight="1">
@@ -539,45 +742,83 @@
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="2"/>
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="2"/>
+      <c r="A11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="2"/>
+      <c r="A12" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="2"/>
+      <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="2"/>
+      <c r="A14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" ht="16.5" customHeight="1">

</xml_diff>

<commit_message>
update note on learning English
</commit_message>
<xml_diff>
--- a/Words/Mispronounced words.xlsx
+++ b/Words/Mispronounced words.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Private Files\English Note\Words\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4EEE620-AB56-4D6D-A72B-745D3C7F63F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E8D4D2-1BD5-44C6-87BB-F98C96C8CCBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Words</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -312,6 +312,15 @@
   </si>
   <si>
     <t>[adj.][n.]</t>
+  </si>
+  <si>
+    <t>vault</t>
+  </si>
+  <si>
+    <t>/vO:lt/</t>
+  </si>
+  <si>
+    <t>vt. vi.</t>
   </si>
 </sst>
 </file>
@@ -719,7 +728,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -922,9 +931,15 @@
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A18" s="1"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="2"/>
+      <c r="A18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" ht="16.5" customHeight="1">

</xml_diff>

<commit_message>
add note on 'In Touch'
</commit_message>
<xml_diff>
--- a/Words/Mispronounced words.xlsx
+++ b/Words/Mispronounced words.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Private Files\English Note\Words\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E8D4D2-1BD5-44C6-87BB-F98C96C8CCBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198DCFFE-5BD8-451B-A868-402DE250EC48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>Words</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -321,6 +321,12 @@
   </si>
   <si>
     <t>vt. vi.</t>
+  </si>
+  <si>
+    <t>festival</t>
+  </si>
+  <si>
+    <t>/'festIvl/</t>
   </si>
 </sst>
 </file>
@@ -728,7 +734,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -943,9 +949,15 @@
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A19" s="1"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="2"/>
+      <c r="A19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" ht="16.5" customHeight="1">

</xml_diff>

<commit_message>
update note on English
</commit_message>
<xml_diff>
--- a/Words/Mispronounced words.xlsx
+++ b/Words/Mispronounced words.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Private Files\English Note\Words\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198DCFFE-5BD8-451B-A868-402DE250EC48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6184433-477B-4AA4-BDAA-CD7488EDC904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>Words</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -245,9 +245,6 @@
     </r>
   </si>
   <si>
-    <t>n.single</t>
-  </si>
-  <si>
     <t>family</t>
   </si>
   <si>
@@ -327,6 +324,18 @@
   </si>
   <si>
     <t>/'festIvl/</t>
+  </si>
+  <si>
+    <t>senator</t>
+  </si>
+  <si>
+    <t>/'senEtE/</t>
+  </si>
+  <si>
+    <t>senate</t>
+  </si>
+  <si>
+    <t>n.Singular</t>
   </si>
 </sst>
 </file>
@@ -734,7 +743,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -898,62 +907,62 @@
         <v>35</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" ht="16.5" customHeight="1">
       <c r="A15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" ht="16.5" customHeight="1">
       <c r="A16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" ht="16.5" customHeight="1">
       <c r="A17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="C17" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" ht="16.5" customHeight="1">
       <c r="A18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="C18" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" ht="16.5" customHeight="1">
       <c r="A19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>49</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>29</v>
@@ -961,15 +970,27 @@
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A20" s="1"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="2"/>
+      <c r="A20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A21" s="1"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="2"/>
+      <c r="A21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" ht="16.5" customHeight="1">

</xml_diff>

<commit_message>
update an essay of task 1 of IELTS
</commit_message>
<xml_diff>
--- a/Words/Mispronounced words.xlsx
+++ b/Words/Mispronounced words.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Private Files\English Note\Words\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A55ABF6-DC9D-4165-9037-CAC92C26E352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E4991B-AA9D-4E41-BD6F-DFCCC9AC97C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="80">
   <si>
     <t>Words</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>part of speech</t>
-  </si>
-  <si>
-    <t>meaning</t>
   </si>
   <si>
     <t>[n.] [v.]</t>
@@ -383,10 +380,25 @@
     <t>swap</t>
   </si>
   <si>
-    <t>/swO:p</t>
-  </si>
-  <si>
     <t>/tE/</t>
+  </si>
+  <si>
+    <t>gnome</t>
+  </si>
+  <si>
+    <t>/swO:p/</t>
+  </si>
+  <si>
+    <t>/nEum/</t>
+  </si>
+  <si>
+    <t>/swQp/</t>
+  </si>
+  <si>
+    <t>g' is silent</t>
+  </si>
+  <si>
+    <t>remark</t>
   </si>
 </sst>
 </file>
@@ -506,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -532,6 +544,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -814,8 +827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -823,6 +836,7 @@
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="3" width="19.42578125" style="5" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" customHeight="1">
@@ -833,13 +847,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>13</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16.5" customHeight="1">
@@ -847,11 +861,11 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="2"/>
     </row>
@@ -897,7 +911,7 @@
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>11</v>
@@ -905,10 +919,10 @@
     </row>
     <row r="7" spans="1:5" ht="16.5" customHeight="1">
       <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
         <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="2"/>
@@ -916,10 +930,10 @@
     </row>
     <row r="8" spans="1:5" ht="16.5" customHeight="1">
       <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="2"/>
@@ -927,10 +941,10 @@
     </row>
     <row r="9" spans="1:5" ht="16.5" customHeight="1">
       <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="2"/>
@@ -938,77 +952,77 @@
     </row>
     <row r="10" spans="1:5" ht="16.5" customHeight="1">
       <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" ht="16.5" customHeight="1">
       <c r="A11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" ht="16.5" customHeight="1">
       <c r="A12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>27</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" ht="16.5" customHeight="1">
       <c r="A13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" ht="16.5" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" ht="16.5" customHeight="1">
       <c r="A15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="2"/>
@@ -1016,194 +1030,204 @@
     </row>
     <row r="16" spans="1:5" ht="16.5" customHeight="1">
       <c r="A16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" ht="16.5" customHeight="1">
       <c r="A17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" ht="16.5" customHeight="1">
       <c r="A18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>44</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" ht="16.5" customHeight="1">
       <c r="A19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>47</v>
-      </c>
       <c r="C19" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" ht="16.5" customHeight="1">
       <c r="A20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>49</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" ht="16.5" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" ht="16.5" customHeight="1">
       <c r="A22" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>51</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>52</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" ht="16.5" customHeight="1">
       <c r="A23" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>53</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>54</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" ht="16.5" customHeight="1">
       <c r="A24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>56</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" ht="16.5" customHeight="1">
       <c r="A25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>62</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>63</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" ht="16.5" customHeight="1">
       <c r="A26" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>65</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>66</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" ht="17.25">
       <c r="A27" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>68</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>69</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5" ht="17.25">
       <c r="A28" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="8" t="s">
         <v>70</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>71</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5" ht="17.25">
       <c r="A29" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B29" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5" ht="17.25">
+      <c r="A30" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E29" s="2"/>
-    </row>
-    <row r="30" spans="1:5" ht="17.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="8"/>
+      <c r="B30" s="8" t="s">
+        <v>76</v>
+      </c>
       <c r="C30" s="8"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
+      <c r="D30" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>78</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
review an IELTS essay and add new words
</commit_message>
<xml_diff>
--- a/Words/Mispronounced words.xlsx
+++ b/Words/Mispronounced words.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Private Files\English Note\Words\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B586BB9-7991-4130-A66D-780F5717BD1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FE8FFE-B39A-4255-A9CE-4BD5AC86FAE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="93">
   <si>
     <t>Words</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -424,6 +424,21 @@
   </si>
   <si>
     <t>/pE'destrIEn/ n. adj.</t>
+  </si>
+  <si>
+    <t>cloth</t>
+  </si>
+  <si>
+    <t>clothe</t>
+  </si>
+  <si>
+    <t>/KlOT/ n.</t>
+  </si>
+  <si>
+    <t>/klEuT/</t>
+  </si>
+  <si>
+    <t>/klED/ vt.</t>
   </si>
 </sst>
 </file>
@@ -575,7 +590,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -611,6 +626,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1307,7 +1323,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1380,15 +1396,25 @@
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A6" s="1"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
+      <c r="A6" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>91</v>
+      </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A7" s="1"/>
-      <c r="B7" s="11"/>
+      <c r="A7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>92</v>
+      </c>
       <c r="C7" s="11"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>

</xml_diff>

<commit_message>
update notes of IELTS
</commit_message>
<xml_diff>
--- a/Words/Mispronounced words.xlsx
+++ b/Words/Mispronounced words.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Private Files\English Note\Words\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9794F040-FC8E-4A02-80C5-E81457688820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CBC58E8-5A1A-4F34-8101-1498BF7DA4A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="103">
   <si>
     <t>Words</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -457,6 +457,18 @@
   </si>
   <si>
     <t>/E'kVrEns/</t>
+  </si>
+  <si>
+    <t>synchronous</t>
+  </si>
+  <si>
+    <t>asynchronous</t>
+  </si>
+  <si>
+    <t>/eI'sINkREnEs/</t>
+  </si>
+  <si>
+    <t>/'sINkrEnEs/</t>
   </si>
 </sst>
 </file>
@@ -608,7 +620,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -646,6 +658,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1342,12 +1355,12 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="19.42578125" style="5" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
@@ -1478,17 +1491,29 @@
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A11" s="1"/>
-      <c r="B11" s="8"/>
+      <c r="A11" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>102</v>
+      </c>
       <c r="C11" s="8"/>
-      <c r="D11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A12" s="6"/>
-      <c r="B12" s="8"/>
+      <c r="A12" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>101</v>
+      </c>
       <c r="C12" s="8"/>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" ht="16.5" customHeight="1">

</xml_diff>

<commit_message>
update words and journals
</commit_message>
<xml_diff>
--- a/Words/Mispronounced words.xlsx
+++ b/Words/Mispronounced words.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Private Files\English Note\Words\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Private Files\English Notes\Words\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CBC58E8-5A1A-4F34-8101-1498BF7DA4A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A16DB83-9E3B-43BE-A66A-7AC7A18FD1DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="105">
   <si>
     <t>Words</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -438,9 +438,6 @@
     <t>/klEuT/</t>
   </si>
   <si>
-    <t>/klED/ vt.</t>
-  </si>
-  <si>
     <t>occur</t>
   </si>
   <si>
@@ -469,13 +466,22 @@
   </si>
   <si>
     <t>/'sINkrEnEs/</t>
+  </si>
+  <si>
+    <t>villain</t>
+  </si>
+  <si>
+    <t>/'vIlEn/</t>
+  </si>
+  <si>
+    <t>/klEuD/ vt.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -533,6 +539,39 @@
       <color rgb="FF1F2328"/>
       <name val="GWIPA"/>
       <charset val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="GWIPA"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="GWIPA"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -620,7 +659,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -650,15 +689,31 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1355,299 +1410,304 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="19.42578125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="5" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="31.5" customHeight="1">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="17" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="15" t="s">
         <v>80</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
     </row>
     <row r="3" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="21" t="s">
         <v>83</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>84</v>
       </c>
       <c r="C3" s="9"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
     </row>
     <row r="4" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A4" s="18"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="14" t="s">
         <v>85</v>
       </c>
       <c r="C4" s="9"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
     </row>
     <row r="5" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="15" t="s">
         <v>86</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
     </row>
     <row r="6" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="15" t="s">
         <v>88</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
     </row>
     <row r="7" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="15" t="s">
         <v>89</v>
       </c>
       <c r="B7" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="24"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+    </row>
+    <row r="8" spans="1:5" ht="16.5" customHeight="1">
+      <c r="A8" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A8" s="1" t="s">
+      <c r="B8" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="C8" s="18"/>
+      <c r="D8" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="20"/>
+    </row>
+    <row r="9" spans="1:5" ht="16.5" customHeight="1">
+      <c r="A9" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="D9" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="20"/>
+    </row>
+    <row r="10" spans="1:5" ht="16.5" customHeight="1">
+      <c r="A10" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A9" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B9" s="8" t="s">
+      <c r="B10" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="18"/>
+      <c r="D10" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="20"/>
+    </row>
+    <row r="11" spans="1:5" ht="16.5" customHeight="1">
+      <c r="A11" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A10" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="20"/>
+    </row>
+    <row r="12" spans="1:5" ht="16.5" customHeight="1">
+      <c r="A12" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B12" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="20"/>
+    </row>
+    <row r="13" spans="1:5" ht="16.5" customHeight="1">
+      <c r="A13" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A12" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="B13" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
     </row>
     <row r="14" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A14" s="1"/>
+      <c r="A14" s="15"/>
       <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
     </row>
     <row r="15" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A15" s="1"/>
+      <c r="A15" s="15"/>
       <c r="B15" s="8"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
     </row>
     <row r="16" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A16" s="1"/>
+      <c r="A16" s="15"/>
       <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
     </row>
     <row r="17" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A17" s="1"/>
+      <c r="A17" s="15"/>
       <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
     </row>
     <row r="18" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A18" s="1"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
     </row>
     <row r="19" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A19" s="1"/>
+      <c r="A19" s="15"/>
       <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
     </row>
     <row r="20" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A20" s="1"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="8"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
     </row>
     <row r="21" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A21" s="1"/>
+      <c r="A21" s="15"/>
       <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
     </row>
     <row r="22" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A22" s="1"/>
+      <c r="A22" s="15"/>
       <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
     </row>
     <row r="23" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A23" s="1"/>
+      <c r="A23" s="15"/>
       <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
     </row>
     <row r="24" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A24" s="1"/>
+      <c r="A24" s="15"/>
       <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
     </row>
     <row r="25" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A25" s="1"/>
+      <c r="A25" s="15"/>
       <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
     </row>
     <row r="26" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A26" s="1"/>
+      <c r="A26" s="15"/>
       <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
     </row>
     <row r="27" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A27" s="2"/>
+      <c r="A27" s="16"/>
       <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:5" ht="17.25">
-      <c r="A28" s="2"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+    </row>
+    <row r="28" spans="1:5" ht="18">
+      <c r="A28" s="16"/>
       <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="1:5" ht="17.25">
-      <c r="A29" s="2"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+    </row>
+    <row r="29" spans="1:5" ht="18">
+      <c r="A29" s="16"/>
       <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-    </row>
-    <row r="30" spans="1:5" ht="17.25">
-      <c r="A30" s="2"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+    </row>
+    <row r="30" spans="1:5" ht="18">
+      <c r="A30" s="16"/>
       <c r="B30" s="8"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="1:5" ht="17.25">
-      <c r="A31" s="2"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+    </row>
+    <row r="31" spans="1:5" ht="18">
+      <c r="A31" s="16"/>
       <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="13"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
anaylysing answers of listening test
</commit_message>
<xml_diff>
--- a/Words/Mispronounced words.xlsx
+++ b/Words/Mispronounced words.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Private Files\English Notes\Words\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094BDD79-363B-498E-BE62-61D57FCE0DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCC197B-C42F-4D8F-B549-134868EBC39E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -740,7 +740,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1434,7 +1434,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
udpate notes of IELTS
</commit_message>
<xml_diff>
--- a/Words/Mispronounced words.xlsx
+++ b/Words/Mispronounced words.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Private Files\English Notes\Words\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCC197B-C42F-4D8F-B549-134868EBC39E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -504,7 +498,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="14">
     <font>
       <sz val="11"/>
@@ -798,7 +792,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -833,7 +827,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -1010,14 +1004,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
@@ -1430,7 +1424,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02EC5A63-60FD-4B67-81C7-9531B7E4CFB3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">

</xml_diff>

<commit_message>
updat notes of listening
</commit_message>
<xml_diff>
--- a/Words/Mispronounced words.xlsx
+++ b/Words/Mispronounced words.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="120">
   <si>
     <t>Words</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -502,6 +502,18 @@
   </si>
   <si>
     <t>"b" is silent.</t>
+  </si>
+  <si>
+    <t>debris</t>
+  </si>
+  <si>
+    <t>/debri:/</t>
+  </si>
+  <si>
+    <t>s' is silent.</t>
+  </si>
+  <si>
+    <t>U.</t>
   </si>
 </sst>
 </file>
@@ -1013,7 +1025,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1437,7 +1449,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1667,11 +1679,19 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A18" s="15"/>
-      <c r="B18" s="8"/>
+      <c r="A18" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>117</v>
+      </c>
       <c r="C18" s="18"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
+      <c r="D18" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="19" spans="1:5" ht="16.5" customHeight="1">
       <c r="A19" s="15"/>

</xml_diff>